<commit_message>
import with lat long
</commit_message>
<xml_diff>
--- a/resources/import/applications/service_directory/services_sample.xlsx
+++ b/resources/import/applications/service_directory/services_sample.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\sportzweb\resources\import\applications\service_directory\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
@@ -10,8 +15,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>address</t>
   </si>
@@ -49,13 +54,19 @@
   </si>
   <si>
     <t>service_category_name</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -359,21 +370,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" style="1" customWidth="1"/>
@@ -388,7 +399,7 @@
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -418,6 +429,12 @@
       </c>
       <c r="J1" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>